<commit_message>
atualizacao dicionarios de dados revisados
</commit_message>
<xml_diff>
--- a/datasets/dicionarios_dados/actividad_fisica_w_adultos.Catalogo_revisado.xlsx
+++ b/datasets/dicionarios_dados/actividad_fisica_w_adultos.Catalogo_revisado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\mvp_analise_exploratoria_2024-09\datasets\dicionarios_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364C2A4D-4552-4EB3-9002-FA539DFFD5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE35783-7FBB-4FDD-9880-7C87B2FFFBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="473">
   <si>
     <t>Etiqueta</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t>Atributo Revisado</t>
+  </si>
+  <si>
+    <t>ext_sel</t>
   </si>
 </sst>
 </file>
@@ -2665,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5153,7 +5156,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="24" t="s">
-        <v>228</v>
+        <v>472</v>
       </c>
       <c r="B126" s="11" t="s">
         <v>228</v>
@@ -5234,7 +5237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A16:C650"/>
   <sheetViews>
-    <sheetView topLeftCell="A638" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A641" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A646" sqref="A646:A650"/>
     </sheetView>
   </sheetViews>

</xml_diff>